<commit_message>
pre-process Shir data for decoding analysis
</commit_message>
<xml_diff>
--- a/inclusion_lists/decoding_exp_list.xlsx
+++ b/inclusion_lists/decoding_exp_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="218">
   <si>
     <t>bat_num</t>
   </si>
@@ -490,6 +490,189 @@
   </si>
   <si>
     <t>b0148_d170807</t>
+  </si>
+  <si>
+    <t>b2382_d190623</t>
+  </si>
+  <si>
+    <t>b2382_d190624</t>
+  </si>
+  <si>
+    <t>b2382_d190625</t>
+  </si>
+  <si>
+    <t>b2382_d190627</t>
+  </si>
+  <si>
+    <t>b2382_d190628</t>
+  </si>
+  <si>
+    <t>b2382_d190630</t>
+  </si>
+  <si>
+    <t>b2382_d190701</t>
+  </si>
+  <si>
+    <t>b2382_d190703</t>
+  </si>
+  <si>
+    <t>b2382_d190707</t>
+  </si>
+  <si>
+    <t>b2382_d190708</t>
+  </si>
+  <si>
+    <t>b2382_d190709</t>
+  </si>
+  <si>
+    <t>b2382_d190712</t>
+  </si>
+  <si>
+    <t>b2382_d190714</t>
+  </si>
+  <si>
+    <t>b2382_d190715</t>
+  </si>
+  <si>
+    <t>b2382_d190716</t>
+  </si>
+  <si>
+    <t>b2382_d190718</t>
+  </si>
+  <si>
+    <t>b2382_d190721</t>
+  </si>
+  <si>
+    <t>b2382_d190722</t>
+  </si>
+  <si>
+    <t>b2382_d190724</t>
+  </si>
+  <si>
+    <t>b2382_d190725</t>
+  </si>
+  <si>
+    <t>b2382_d190728</t>
+  </si>
+  <si>
+    <t>b2382_d190729</t>
+  </si>
+  <si>
+    <t>b2382_d190730</t>
+  </si>
+  <si>
+    <t>b2382_d190731</t>
+  </si>
+  <si>
+    <t>b2382_d190801</t>
+  </si>
+  <si>
+    <t>b2382_d190804</t>
+  </si>
+  <si>
+    <t>b2382_d190805</t>
+  </si>
+  <si>
+    <t>b2382_d190807</t>
+  </si>
+  <si>
+    <t>b2382_d190808</t>
+  </si>
+  <si>
+    <t>b2382_d190811</t>
+  </si>
+  <si>
+    <t>b2382_d190812</t>
+  </si>
+  <si>
+    <t>b2382_d190813</t>
+  </si>
+  <si>
+    <t>b2382_d190814</t>
+  </si>
+  <si>
+    <t>b0194_d180429</t>
+  </si>
+  <si>
+    <t>b0194_d180501</t>
+  </si>
+  <si>
+    <t>b0194_d180502</t>
+  </si>
+  <si>
+    <t>b0194_d180503</t>
+  </si>
+  <si>
+    <t>b0194_d180505</t>
+  </si>
+  <si>
+    <t>b0194_d180507</t>
+  </si>
+  <si>
+    <t>b0194_d180508</t>
+  </si>
+  <si>
+    <t>b0194_d180509</t>
+  </si>
+  <si>
+    <t>b0194_d180510</t>
+  </si>
+  <si>
+    <t>b0194_d180513</t>
+  </si>
+  <si>
+    <t>b0194_d180514</t>
+  </si>
+  <si>
+    <t>b0194_d180515</t>
+  </si>
+  <si>
+    <t>b0194_d180516</t>
+  </si>
+  <si>
+    <t>b0194_d180520</t>
+  </si>
+  <si>
+    <t>b0194_d180521</t>
+  </si>
+  <si>
+    <t>b0194_d180522</t>
+  </si>
+  <si>
+    <t>b0194_d180528</t>
+  </si>
+  <si>
+    <t>b0194_d180531</t>
+  </si>
+  <si>
+    <t>b0194_d180604</t>
+  </si>
+  <si>
+    <t>b0194_d180605</t>
+  </si>
+  <si>
+    <t>b0194_d180606</t>
+  </si>
+  <si>
+    <t>b0194_d180607</t>
+  </si>
+  <si>
+    <t>b0194_d180610</t>
+  </si>
+  <si>
+    <t>b0194_d180611</t>
+  </si>
+  <si>
+    <t>b0194_d180612</t>
+  </si>
+  <si>
+    <t>b0194_d180614</t>
+  </si>
+  <si>
+    <t>over-representation only at the very last bin</t>
+  </si>
+  <si>
+    <t>need to process this day</t>
   </si>
 </sst>
 </file>
@@ -525,8 +708,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,11 +993,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D209"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="C150" sqref="C150"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -820,14 +1004,14 @@
     <col min="4" max="4" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>117</v>
       </c>
       <c r="D1" t="s">
@@ -2431,7 +2615,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>151</v>
       </c>
@@ -2442,7 +2626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>152</v>
       </c>
@@ -2453,7 +2637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>153</v>
       </c>
@@ -2464,7 +2648,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>154</v>
       </c>
@@ -2475,7 +2659,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>155</v>
       </c>
@@ -2486,7 +2670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>156</v>
       </c>
@@ -2494,6 +2678,688 @@
         <v>148</v>
       </c>
       <c r="C150">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>157</v>
+      </c>
+      <c r="B151">
+        <v>2382</v>
+      </c>
+      <c r="C151">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>158</v>
+      </c>
+      <c r="B152">
+        <v>2382</v>
+      </c>
+      <c r="C152">
+        <v>0.5</v>
+      </c>
+      <c r="D152" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>159</v>
+      </c>
+      <c r="B153">
+        <v>2382</v>
+      </c>
+      <c r="C153">
+        <v>0.5</v>
+      </c>
+      <c r="D153" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>160</v>
+      </c>
+      <c r="B154">
+        <v>2382</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>161</v>
+      </c>
+      <c r="B155">
+        <v>2382</v>
+      </c>
+      <c r="C155">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>162</v>
+      </c>
+      <c r="B156">
+        <v>2382</v>
+      </c>
+      <c r="C156">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>163</v>
+      </c>
+      <c r="B157">
+        <v>2382</v>
+      </c>
+      <c r="C157">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" t="s">
+        <v>164</v>
+      </c>
+      <c r="B158">
+        <v>2382</v>
+      </c>
+      <c r="C158">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>165</v>
+      </c>
+      <c r="B159">
+        <v>2382</v>
+      </c>
+      <c r="C159">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>166</v>
+      </c>
+      <c r="B160">
+        <v>2382</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>167</v>
+      </c>
+      <c r="B161">
+        <v>2382</v>
+      </c>
+      <c r="C161">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A162" t="s">
+        <v>168</v>
+      </c>
+      <c r="B162">
+        <v>2382</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>169</v>
+      </c>
+      <c r="B163">
+        <v>2382</v>
+      </c>
+      <c r="C163">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>170</v>
+      </c>
+      <c r="B164">
+        <v>2382</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>171</v>
+      </c>
+      <c r="B165">
+        <v>2382</v>
+      </c>
+      <c r="C165">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>172</v>
+      </c>
+      <c r="B166">
+        <v>2382</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>173</v>
+      </c>
+      <c r="B167">
+        <v>2382</v>
+      </c>
+      <c r="C167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>174</v>
+      </c>
+      <c r="B168">
+        <v>2382</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>175</v>
+      </c>
+      <c r="B169">
+        <v>2382</v>
+      </c>
+      <c r="C169">
+        <v>0.5</v>
+      </c>
+      <c r="D169" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A170" t="s">
+        <v>176</v>
+      </c>
+      <c r="B170">
+        <v>2382</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>177</v>
+      </c>
+      <c r="B171">
+        <v>2382</v>
+      </c>
+      <c r="C171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
+        <v>178</v>
+      </c>
+      <c r="B172">
+        <v>2382</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>179</v>
+      </c>
+      <c r="B173">
+        <v>2382</v>
+      </c>
+      <c r="C173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A174" t="s">
+        <v>180</v>
+      </c>
+      <c r="B174">
+        <v>2382</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>181</v>
+      </c>
+      <c r="B175">
+        <v>2382</v>
+      </c>
+      <c r="C175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A176" t="s">
+        <v>182</v>
+      </c>
+      <c r="B176">
+        <v>2382</v>
+      </c>
+      <c r="C176">
+        <v>0.5</v>
+      </c>
+      <c r="D176" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>183</v>
+      </c>
+      <c r="B177">
+        <v>2382</v>
+      </c>
+      <c r="C177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>184</v>
+      </c>
+      <c r="B178">
+        <v>2382</v>
+      </c>
+      <c r="C178">
+        <v>0.5</v>
+      </c>
+      <c r="D178" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>185</v>
+      </c>
+      <c r="B179">
+        <v>2382</v>
+      </c>
+      <c r="C179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A180" t="s">
+        <v>186</v>
+      </c>
+      <c r="B180">
+        <v>2382</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>187</v>
+      </c>
+      <c r="B181">
+        <v>2382</v>
+      </c>
+      <c r="C181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" t="s">
+        <v>188</v>
+      </c>
+      <c r="B182">
+        <v>2382</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>189</v>
+      </c>
+      <c r="B183">
+        <v>2382</v>
+      </c>
+      <c r="C183">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A184" t="s">
+        <v>190</v>
+      </c>
+      <c r="B184">
+        <v>194</v>
+      </c>
+      <c r="D184" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>191</v>
+      </c>
+      <c r="B185">
+        <v>194</v>
+      </c>
+      <c r="C185">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>192</v>
+      </c>
+      <c r="B186">
+        <v>194</v>
+      </c>
+      <c r="C186">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>193</v>
+      </c>
+      <c r="B187">
+        <v>194</v>
+      </c>
+      <c r="C187">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>194</v>
+      </c>
+      <c r="B188">
+        <v>194</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>195</v>
+      </c>
+      <c r="B189">
+        <v>194</v>
+      </c>
+      <c r="C189">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>196</v>
+      </c>
+      <c r="B190">
+        <v>194</v>
+      </c>
+      <c r="C190">
+        <v>0.5</v>
+      </c>
+      <c r="D190" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>197</v>
+      </c>
+      <c r="B191">
+        <v>194</v>
+      </c>
+      <c r="C191">
+        <v>0.5</v>
+      </c>
+      <c r="D191" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" t="s">
+        <v>198</v>
+      </c>
+      <c r="B192">
+        <v>194</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>199</v>
+      </c>
+      <c r="B193">
+        <v>194</v>
+      </c>
+      <c r="C193">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194">
+        <v>194</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>201</v>
+      </c>
+      <c r="B195">
+        <v>194</v>
+      </c>
+      <c r="C195">
+        <v>0.5</v>
+      </c>
+      <c r="D195" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" t="s">
+        <v>202</v>
+      </c>
+      <c r="B196">
+        <v>194</v>
+      </c>
+      <c r="C196">
+        <v>0.5</v>
+      </c>
+      <c r="D196" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>203</v>
+      </c>
+      <c r="B197">
+        <v>194</v>
+      </c>
+      <c r="C197">
+        <v>0.5</v>
+      </c>
+      <c r="D197" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" t="s">
+        <v>204</v>
+      </c>
+      <c r="B198">
+        <v>194</v>
+      </c>
+      <c r="C198">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>205</v>
+      </c>
+      <c r="B199">
+        <v>194</v>
+      </c>
+      <c r="C199">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" t="s">
+        <v>206</v>
+      </c>
+      <c r="B200">
+        <v>194</v>
+      </c>
+      <c r="C200">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="201" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>207</v>
+      </c>
+      <c r="B201">
+        <v>194</v>
+      </c>
+      <c r="C201">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>208</v>
+      </c>
+      <c r="B202">
+        <v>194</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>209</v>
+      </c>
+      <c r="B203">
+        <v>194</v>
+      </c>
+      <c r="C203">
+        <v>0.5</v>
+      </c>
+      <c r="D203" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" t="s">
+        <v>210</v>
+      </c>
+      <c r="B204">
+        <v>194</v>
+      </c>
+      <c r="C204">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>211</v>
+      </c>
+      <c r="B205">
+        <v>194</v>
+      </c>
+      <c r="C205">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" t="s">
+        <v>212</v>
+      </c>
+      <c r="B206">
+        <v>194</v>
+      </c>
+      <c r="C206">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>213</v>
+      </c>
+      <c r="B207">
+        <v>194</v>
+      </c>
+      <c r="C207">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" t="s">
+        <v>214</v>
+      </c>
+      <c r="B208">
+        <v>194</v>
+      </c>
+      <c r="C208">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>215</v>
+      </c>
+      <c r="B209">
+        <v>194</v>
+      </c>
+      <c r="C209">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
making order in shir data
</commit_message>
<xml_diff>
--- a/inclusion_lists/decoding_exp_list.xlsx
+++ b/inclusion_lists/decoding_exp_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="253">
   <si>
     <t>bat_num</t>
   </si>
@@ -673,6 +673,111 @@
   </si>
   <si>
     <t>need to process this day</t>
+  </si>
+  <si>
+    <t>b9845_d170212</t>
+  </si>
+  <si>
+    <t>b9845_d170215</t>
+  </si>
+  <si>
+    <t>b9845_d170216</t>
+  </si>
+  <si>
+    <t>b9845_d170217</t>
+  </si>
+  <si>
+    <t>b9845_d170219</t>
+  </si>
+  <si>
+    <t>b9845_d170220</t>
+  </si>
+  <si>
+    <t>b9845_d170221</t>
+  </si>
+  <si>
+    <t>b9845_d170222</t>
+  </si>
+  <si>
+    <t>b9845_d170223</t>
+  </si>
+  <si>
+    <t>b9845_d170516</t>
+  </si>
+  <si>
+    <t>b9845_d170517</t>
+  </si>
+  <si>
+    <t>b9845_d170518</t>
+  </si>
+  <si>
+    <t>b9845_d170525</t>
+  </si>
+  <si>
+    <t>b9845_d170527</t>
+  </si>
+  <si>
+    <t>b9845_d170528</t>
+  </si>
+  <si>
+    <t>b9845_d170529</t>
+  </si>
+  <si>
+    <t>b9845_d170603</t>
+  </si>
+  <si>
+    <t>b9845_d170605</t>
+  </si>
+  <si>
+    <t>b9845_d170606</t>
+  </si>
+  <si>
+    <t>b9845_d170612</t>
+  </si>
+  <si>
+    <t>b9845_d170614</t>
+  </si>
+  <si>
+    <t>b9845_d170622</t>
+  </si>
+  <si>
+    <t>b2311_d191218</t>
+  </si>
+  <si>
+    <t>b2311_d191219</t>
+  </si>
+  <si>
+    <t>b2311_d191220</t>
+  </si>
+  <si>
+    <t>b2311_d191222</t>
+  </si>
+  <si>
+    <t>b2311_d191223</t>
+  </si>
+  <si>
+    <t>b2311_d191224</t>
+  </si>
+  <si>
+    <t>b2311_d191225</t>
+  </si>
+  <si>
+    <t>b2311_d191226</t>
+  </si>
+  <si>
+    <t>b2311_d191229</t>
+  </si>
+  <si>
+    <t>b2311_d191230</t>
+  </si>
+  <si>
+    <t>b2311_d191231</t>
+  </si>
+  <si>
+    <t>b2311_d200101</t>
+  </si>
+  <si>
+    <t>b2311_d200102</t>
   </si>
 </sst>
 </file>
@@ -993,9 +1098,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D209"/>
+  <dimension ref="A1:D244"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A208" workbookViewId="0">
+      <selection activeCell="A245" sqref="A245"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3363,6 +3470,391 @@
         <v>0</v>
       </c>
     </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" t="s">
+        <v>218</v>
+      </c>
+      <c r="B210">
+        <v>9845</v>
+      </c>
+      <c r="C210">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>219</v>
+      </c>
+      <c r="B211">
+        <v>9845</v>
+      </c>
+      <c r="C211">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" t="s">
+        <v>220</v>
+      </c>
+      <c r="B212">
+        <v>9845</v>
+      </c>
+      <c r="C212">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>221</v>
+      </c>
+      <c r="B213">
+        <v>9845</v>
+      </c>
+      <c r="C213">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" t="s">
+        <v>222</v>
+      </c>
+      <c r="B214">
+        <v>9845</v>
+      </c>
+      <c r="C214">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>223</v>
+      </c>
+      <c r="B215">
+        <v>9845</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" t="s">
+        <v>224</v>
+      </c>
+      <c r="B216">
+        <v>9845</v>
+      </c>
+      <c r="C216">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>225</v>
+      </c>
+      <c r="B217">
+        <v>9845</v>
+      </c>
+      <c r="C217">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" t="s">
+        <v>226</v>
+      </c>
+      <c r="B218">
+        <v>9845</v>
+      </c>
+      <c r="C218">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>227</v>
+      </c>
+      <c r="B219">
+        <v>9845</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" t="s">
+        <v>228</v>
+      </c>
+      <c r="B220">
+        <v>9845</v>
+      </c>
+      <c r="C220">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>229</v>
+      </c>
+      <c r="B221">
+        <v>9845</v>
+      </c>
+      <c r="C221">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" t="s">
+        <v>230</v>
+      </c>
+      <c r="B222">
+        <v>9845</v>
+      </c>
+      <c r="C222">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>231</v>
+      </c>
+      <c r="B223">
+        <v>9845</v>
+      </c>
+      <c r="C223">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" t="s">
+        <v>232</v>
+      </c>
+      <c r="B224">
+        <v>9845</v>
+      </c>
+      <c r="C224">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>233</v>
+      </c>
+      <c r="B225">
+        <v>9845</v>
+      </c>
+      <c r="C225">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" t="s">
+        <v>234</v>
+      </c>
+      <c r="B226">
+        <v>9845</v>
+      </c>
+      <c r="C226">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>235</v>
+      </c>
+      <c r="B227">
+        <v>9845</v>
+      </c>
+      <c r="C227">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" t="s">
+        <v>236</v>
+      </c>
+      <c r="B228">
+        <v>9845</v>
+      </c>
+      <c r="C228">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>237</v>
+      </c>
+      <c r="B229">
+        <v>9845</v>
+      </c>
+      <c r="C229">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" t="s">
+        <v>238</v>
+      </c>
+      <c r="B230">
+        <v>9845</v>
+      </c>
+      <c r="C230">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>239</v>
+      </c>
+      <c r="B231">
+        <v>9845</v>
+      </c>
+      <c r="C231">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" t="s">
+        <v>240</v>
+      </c>
+      <c r="B232">
+        <v>2311</v>
+      </c>
+      <c r="C232">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>241</v>
+      </c>
+      <c r="B233">
+        <v>2311</v>
+      </c>
+      <c r="C233">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" t="s">
+        <v>242</v>
+      </c>
+      <c r="B234">
+        <v>2311</v>
+      </c>
+      <c r="C234">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>243</v>
+      </c>
+      <c r="B235">
+        <v>2311</v>
+      </c>
+      <c r="C235">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" t="s">
+        <v>244</v>
+      </c>
+      <c r="B236">
+        <v>2311</v>
+      </c>
+      <c r="C236">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>245</v>
+      </c>
+      <c r="B237">
+        <v>2311</v>
+      </c>
+      <c r="C237">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" t="s">
+        <v>246</v>
+      </c>
+      <c r="B238">
+        <v>2311</v>
+      </c>
+      <c r="C238">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>247</v>
+      </c>
+      <c r="B239">
+        <v>2311</v>
+      </c>
+      <c r="C239">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" t="s">
+        <v>248</v>
+      </c>
+      <c r="B240">
+        <v>2311</v>
+      </c>
+      <c r="C240">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>249</v>
+      </c>
+      <c r="B241">
+        <v>2311</v>
+      </c>
+      <c r="C241">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" t="s">
+        <v>250</v>
+      </c>
+      <c r="B242">
+        <v>2311</v>
+      </c>
+      <c r="C242">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>251</v>
+      </c>
+      <c r="B243">
+        <v>2311</v>
+      </c>
+      <c r="C243">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" t="s">
+        <v>252</v>
+      </c>
+      <c r="B244">
+        <v>2311</v>
+      </c>
+      <c r="C244">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B2:D120">
     <sortCondition ref="B1"/>

</xml_diff>